<commit_message>
typos in species names
</commit_message>
<xml_diff>
--- a/Data/TABLE_S3_COM3_NEW_prMW.xlsx
+++ b/Data/TABLE_S3_COM3_NEW_prMW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A3FD2-C4CA-4414-83D0-3DE67D273A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8136DE-2B2E-427B-9BC4-5EE9E4E3D491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3104,27 +3104,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> aff sp. 5 gen 1 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Pichia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve"> aff. sp. 6</t>
     </r>
   </si>
@@ -4464,6 +4443,27 @@
   </si>
   <si>
     <t>Candida railensis</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Pichia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> aff. sp. 5 gen 1 </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5466,26 +5466,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="40.296875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="5.796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="78.296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="40.25" style="1" customWidth="1"/>
+    <col min="2" max="5" width="5.75" style="3" customWidth="1"/>
+    <col min="6" max="6" width="78.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="3" customWidth="1"/>
     <col min="9" max="9" width="46" style="4" customWidth="1"/>
-    <col min="10" max="11" width="11.796875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="36.296875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.796875" style="1"/>
+    <col min="10" max="11" width="11.75" style="1" customWidth="1"/>
+    <col min="12" max="12" width="36.25" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="52.95" customHeight="1">
+    <row r="1" spans="1:12" ht="52.9" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -5501,22 +5501,22 @@
     </row>
     <row r="2" spans="1:12" ht="99" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>437</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>331</v>
@@ -5534,10 +5534,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="16.95" customHeight="1">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16.899999999999999" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>336</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>316</v>
@@ -5575,7 +5575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.05" customHeight="1">
+    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>337</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>320</v>
@@ -5618,7 +5618,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>12</v>
@@ -5648,7 +5648,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>321</v>
@@ -5678,7 +5678,7 @@
         <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>322</v>
@@ -5713,7 +5713,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>17</v>
@@ -5743,7 +5743,7 @@
         <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>22</v>
@@ -5755,7 +5755,7 @@
         <v>100</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5773,7 +5773,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>20</v>
@@ -5785,7 +5785,7 @@
         <v>100</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5803,7 +5803,7 @@
         <v>23</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>24</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="12" spans="1:12" s="18" customFormat="1">
       <c r="A12" s="23" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="14"/>
@@ -5835,7 +5835,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>319</v>
@@ -5847,7 +5847,7 @@
         <v>100</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5868,7 +5868,7 @@
         <v>26</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>27</v>
@@ -5898,7 +5898,7 @@
         <v>29</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>30</v>
@@ -5928,7 +5928,7 @@
         <v>31</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>32</v>
@@ -5966,7 +5966,7 @@
         <v>37</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>38</v>
@@ -5981,7 +5981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="34.950000000000003" customHeight="1">
+    <row r="17" spans="1:12" ht="34.9" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>345</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>36</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>323</v>
@@ -6010,7 +6010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="34.049999999999997" customHeight="1">
+    <row r="18" spans="1:12" ht="34.15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>346</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>34</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>324</v>
@@ -6057,7 +6057,7 @@
         <v>39</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>40</v>
@@ -6069,7 +6069,7 @@
         <v>100</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6089,7 +6089,7 @@
         <v>41</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>325</v>
@@ -6101,7 +6101,7 @@
         <v>100</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6118,7 +6118,7 @@
         <v>42</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>43</v>
@@ -6148,7 +6148,7 @@
         <v>47</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>326</v>
@@ -6178,7 +6178,7 @@
         <v>45</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>46</v>
@@ -6208,7 +6208,7 @@
         <v>48</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>327</v>
@@ -6240,7 +6240,7 @@
         <v>49</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>50</v>
@@ -6252,7 +6252,7 @@
         <v>100</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -6269,7 +6269,7 @@
         <v>53</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>54</v>
@@ -6301,7 +6301,7 @@
         <v>51</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>328</v>
@@ -6316,7 +6316,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16.95" customHeight="1">
+    <row r="28" spans="1:12" ht="16.899999999999999" customHeight="1">
       <c r="A28" s="27" t="s">
         <v>318</v>
       </c>
@@ -6334,10 +6334,10 @@
       </c>
       <c r="I28" s="28"/>
       <c r="L28" s="25" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="16.95" customHeight="1">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="16.899999999999999" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>351</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>59</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>329</v>
@@ -6367,7 +6367,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="34.049999999999997" customHeight="1">
+    <row r="30" spans="1:12" ht="34.15" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>352</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>55</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>330</v>
@@ -6410,7 +6410,7 @@
         <v>57</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>58</v>
@@ -6443,7 +6443,7 @@
         <v>63</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I32" s="21" t="s">
         <v>64</v>
@@ -6455,7 +6455,7 @@
         <v>100</v>
       </c>
       <c r="L32" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -6473,7 +6473,7 @@
         <v>65</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I33" s="21" t="s">
         <v>66</v>
@@ -6485,7 +6485,7 @@
         <v>100</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -6505,7 +6505,7 @@
         <v>67</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I34" s="21" t="s">
         <v>68</v>
@@ -6517,7 +6517,7 @@
         <v>100</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -6535,7 +6535,7 @@
         <v>69</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I35" s="21" t="s">
         <v>70</v>
@@ -6547,7 +6547,7 @@
         <v>100</v>
       </c>
       <c r="L35" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -6568,7 +6568,7 @@
         <v>62</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I36" s="21" t="s">
         <v>61</v>
@@ -6580,7 +6580,7 @@
         <v>100</v>
       </c>
       <c r="L36" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -6601,7 +6601,7 @@
         <v>60</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I37" s="21" t="s">
         <v>61</v>
@@ -6613,7 +6613,7 @@
         <v>100</v>
       </c>
       <c r="L37" s="18" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -6636,7 +6636,7 @@
         <v>71</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I38" s="21" t="s">
         <v>72</v>
@@ -6648,7 +6648,7 @@
         <v>100</v>
       </c>
       <c r="L38" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -6665,7 +6665,7 @@
         <v>73</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I39" s="21" t="s">
         <v>72</v>
@@ -6677,7 +6677,7 @@
         <v>100</v>
       </c>
       <c r="L39" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -6697,7 +6697,7 @@
         <v>74</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I40" s="21" t="s">
         <v>72</v>
@@ -6709,7 +6709,7 @@
         <v>100</v>
       </c>
       <c r="L40" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -6732,7 +6732,7 @@
         <v>75</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>72</v>
@@ -6744,7 +6744,7 @@
         <v>100</v>
       </c>
       <c r="L41" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -6767,7 +6767,7 @@
         <v>76</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I42" s="21" t="s">
         <v>72</v>
@@ -6779,7 +6779,7 @@
         <v>100</v>
       </c>
       <c r="L42" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -6802,7 +6802,7 @@
         <v>77</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>72</v>
@@ -6814,7 +6814,7 @@
         <v>100</v>
       </c>
       <c r="L43" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -6837,7 +6837,7 @@
         <v>78</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I44" s="21" t="s">
         <v>72</v>
@@ -6849,12 +6849,12 @@
         <v>100</v>
       </c>
       <c r="L44" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="18" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C45" s="15">
         <v>9</v>
@@ -6872,7 +6872,7 @@
         <v>79</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>72</v>
@@ -6884,12 +6884,12 @@
         <v>100</v>
       </c>
       <c r="L45" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C46" s="14"/>
       <c r="E46" s="7">
@@ -6902,7 +6902,7 @@
         <v>80</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>72</v>
@@ -6914,7 +6914,7 @@
         <v>100</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -6932,7 +6932,7 @@
         <v>81</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I47" s="21" t="s">
         <v>72</v>
@@ -6944,7 +6944,7 @@
         <v>100</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -6967,7 +6967,7 @@
         <v>82</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I48" s="21" t="s">
         <v>72</v>
@@ -6979,7 +6979,7 @@
         <v>100</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -7000,7 +7000,7 @@
         <v>83</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I49" s="21" t="s">
         <v>72</v>
@@ -7012,7 +7012,7 @@
         <v>100</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -7030,7 +7030,7 @@
         <v>84</v>
       </c>
       <c r="H50" s="19" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I50" s="21" t="s">
         <v>72</v>
@@ -7042,7 +7042,7 @@
         <v>100</v>
       </c>
       <c r="L50" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -7065,7 +7065,7 @@
         <v>85</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I51" s="21" t="s">
         <v>72</v>
@@ -7077,7 +7077,7 @@
         <v>100</v>
       </c>
       <c r="L51" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -7098,7 +7098,7 @@
         <v>86</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I52" s="21" t="s">
         <v>72</v>
@@ -7110,7 +7110,7 @@
         <v>100</v>
       </c>
       <c r="L52" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -7128,7 +7128,7 @@
         <v>87</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I53" s="21" t="s">
         <v>72</v>
@@ -7140,7 +7140,7 @@
         <v>100</v>
       </c>
       <c r="L53" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -7158,7 +7158,7 @@
         <v>88</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I54" s="21" t="s">
         <v>72</v>
@@ -7170,7 +7170,7 @@
         <v>100</v>
       </c>
       <c r="L54" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -7188,7 +7188,7 @@
         <v>89</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I55" s="21" t="s">
         <v>72</v>
@@ -7200,7 +7200,7 @@
         <v>96</v>
       </c>
       <c r="L55" s="18" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -7218,7 +7218,7 @@
         <v>90</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>91</v>
@@ -7250,7 +7250,7 @@
         <v>93</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>94</v>
@@ -7267,20 +7267,20 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B58" s="7">
         <v>2</v>
       </c>
       <c r="C58" s="14"/>
       <c r="F58" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>9</v>
@@ -7310,7 +7310,7 @@
         <v>96</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>97</v>
@@ -7327,7 +7327,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="18" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C60" s="15">
         <v>1</v>
@@ -7337,13 +7337,13 @@
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G60" s="18" t="s">
         <v>111</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I60" s="21" t="s">
         <v>112</v>
@@ -7355,12 +7355,12 @@
         <v>100</v>
       </c>
       <c r="L60" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="18" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="7">
@@ -7368,13 +7368,13 @@
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G61" s="18" t="s">
         <v>113</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I61" s="21" t="s">
         <v>112</v>
@@ -7386,7 +7386,7 @@
         <v>100</v>
       </c>
       <c r="L61" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -7405,7 +7405,7 @@
         <v>99</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I62" s="21" t="s">
         <v>100</v>
@@ -7417,7 +7417,7 @@
         <v>97</v>
       </c>
       <c r="L62" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -7435,7 +7435,7 @@
         <v>116</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I63" s="21" t="s">
         <v>109</v>
@@ -7447,7 +7447,7 @@
         <v>99</v>
       </c>
       <c r="L63" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -7468,7 +7468,7 @@
         <v>108</v>
       </c>
       <c r="H64" s="19" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I64" s="21" t="s">
         <v>109</v>
@@ -7480,7 +7480,7 @@
         <v>98</v>
       </c>
       <c r="L64" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -7498,7 +7498,7 @@
         <v>101</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I65" s="21" t="s">
         <v>102</v>
@@ -7510,7 +7510,7 @@
         <v>98</v>
       </c>
       <c r="L65" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -7531,7 +7531,7 @@
         <v>103</v>
       </c>
       <c r="H66" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>102</v>
@@ -7543,7 +7543,7 @@
         <v>98</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -7564,7 +7564,7 @@
         <v>110</v>
       </c>
       <c r="H67" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I67" s="21" t="s">
         <v>102</v>
@@ -7576,7 +7576,7 @@
         <v>98</v>
       </c>
       <c r="L67" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -7597,7 +7597,7 @@
         <v>114</v>
       </c>
       <c r="H68" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I68" s="21" t="s">
         <v>102</v>
@@ -7609,7 +7609,7 @@
         <v>98</v>
       </c>
       <c r="L68" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -7627,7 +7627,7 @@
         <v>104</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I69" s="21" t="s">
         <v>105</v>
@@ -7639,7 +7639,7 @@
         <v>98</v>
       </c>
       <c r="L69" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -7660,7 +7660,7 @@
         <v>106</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I70" s="21" t="s">
         <v>107</v>
@@ -7672,7 +7672,7 @@
         <v>98</v>
       </c>
       <c r="L70" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -7691,7 +7691,7 @@
         <v>115</v>
       </c>
       <c r="H71" s="19" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I71" s="21" t="s">
         <v>107</v>
@@ -7703,7 +7703,7 @@
         <v>100</v>
       </c>
       <c r="L71" s="18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -7724,7 +7724,7 @@
         <v>117</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>118</v>
@@ -7757,7 +7757,7 @@
         <v>122</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>123</v>
@@ -7790,7 +7790,7 @@
         <v>120</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>121</v>
@@ -7820,7 +7820,7 @@
         <v>124</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>125</v>
@@ -7850,7 +7850,7 @@
         <v>127</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>128</v>
@@ -7880,7 +7880,7 @@
         <v>131</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>132</v>
@@ -7897,7 +7897,7 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B78" s="9">
         <v>1</v>
@@ -7912,13 +7912,13 @@
         <v>4</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>134</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>135</v>
@@ -7947,7 +7947,7 @@
         <v>136</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>137</v>
@@ -7977,7 +7977,7 @@
         <v>138</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>139</v>
@@ -7992,7 +7992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:41" ht="31.2">
+    <row r="81" spans="1:41" ht="31.5">
       <c r="A81" s="1" t="s">
         <v>389</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>133</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>334</v>
@@ -8039,7 +8039,7 @@
         <v>140</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I82" s="4" t="s">
         <v>141</v>
@@ -8069,10 +8069,10 @@
         <v>129</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J83" s="1">
         <v>100</v>
@@ -8099,7 +8099,7 @@
         <v>142</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I84" s="4" t="s">
         <v>143</v>
@@ -8116,7 +8116,7 @@
     </row>
     <row r="85" spans="1:41" s="18" customFormat="1">
       <c r="A85" s="23" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="14"/>
@@ -8127,13 +8127,13 @@
         <v>3</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G85" s="18" t="s">
         <v>2</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I85" s="21" t="s">
         <v>3</v>
@@ -8145,7 +8145,7 @@
         <v>100</v>
       </c>
       <c r="L85" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="M85" s="26"/>
       <c r="N85" s="26"/>
@@ -8195,7 +8195,7 @@
         <v>191</v>
       </c>
       <c r="H86" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I86" s="21" t="s">
         <v>192</v>
@@ -8207,7 +8207,7 @@
         <v>100</v>
       </c>
       <c r="L86" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="87" spans="1:41">
@@ -8230,7 +8230,7 @@
         <v>179</v>
       </c>
       <c r="H87" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I87" s="21" t="s">
         <v>180</v>
@@ -8242,7 +8242,7 @@
         <v>100</v>
       </c>
       <c r="L87" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:41">
@@ -8260,7 +8260,7 @@
         <v>171</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I88" s="21" t="s">
         <v>172</v>
@@ -8272,7 +8272,7 @@
         <v>100</v>
       </c>
       <c r="L88" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="89" spans="1:41">
@@ -8295,7 +8295,7 @@
         <v>190</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I89" s="21" t="s">
         <v>180</v>
@@ -8307,7 +8307,7 @@
         <v>100</v>
       </c>
       <c r="L89" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="90" spans="1:41">
@@ -8330,7 +8330,7 @@
         <v>183</v>
       </c>
       <c r="H90" s="19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I90" s="21" t="s">
         <v>182</v>
@@ -8342,7 +8342,7 @@
         <v>95</v>
       </c>
       <c r="L90" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="91" spans="1:41">
@@ -8365,7 +8365,7 @@
         <v>181</v>
       </c>
       <c r="H91" s="19" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I91" s="21" t="s">
         <v>182</v>
@@ -8377,7 +8377,7 @@
         <v>95</v>
       </c>
       <c r="L91" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="92" spans="1:41">
@@ -8395,7 +8395,7 @@
         <v>184</v>
       </c>
       <c r="H92" s="19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I92" s="21" t="s">
         <v>182</v>
@@ -8407,7 +8407,7 @@
         <v>95</v>
       </c>
       <c r="L92" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="93" spans="1:41">
@@ -8424,7 +8424,7 @@
         <v>185</v>
       </c>
       <c r="H93" s="19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I93" s="21" t="s">
         <v>182</v>
@@ -8436,7 +8436,7 @@
         <v>95</v>
       </c>
       <c r="L93" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="94" spans="1:41">
@@ -8454,7 +8454,7 @@
         <v>186</v>
       </c>
       <c r="H94" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I94" s="21" t="s">
         <v>182</v>
@@ -8466,7 +8466,7 @@
         <v>95</v>
       </c>
       <c r="L94" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="95" spans="1:41">
@@ -8484,7 +8484,7 @@
         <v>187</v>
       </c>
       <c r="H95" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I95" s="21" t="s">
         <v>182</v>
@@ -8496,7 +8496,7 @@
         <v>95</v>
       </c>
       <c r="L95" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="96" spans="1:41">
@@ -8517,7 +8517,7 @@
         <v>164</v>
       </c>
       <c r="H96" s="19" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I96" s="21" t="s">
         <v>165</v>
@@ -8529,7 +8529,7 @@
         <v>100</v>
       </c>
       <c r="L96" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -8549,7 +8549,7 @@
         <v>193</v>
       </c>
       <c r="H97" s="19" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I97" s="21" t="s">
         <v>148</v>
@@ -8561,7 +8561,7 @@
         <v>100</v>
       </c>
       <c r="L97" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -8579,7 +8579,7 @@
         <v>201</v>
       </c>
       <c r="H98" s="19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I98" s="21" t="s">
         <v>148</v>
@@ -8591,7 +8591,7 @@
         <v>100</v>
       </c>
       <c r="L98" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -8609,7 +8609,7 @@
         <v>196</v>
       </c>
       <c r="H99" s="19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I99" s="21" t="s">
         <v>148</v>
@@ -8621,7 +8621,7 @@
         <v>100</v>
       </c>
       <c r="L99" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -8639,7 +8639,7 @@
         <v>147</v>
       </c>
       <c r="H100" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I100" s="21" t="s">
         <v>148</v>
@@ -8651,7 +8651,7 @@
         <v>100</v>
       </c>
       <c r="L100" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -8669,7 +8669,7 @@
         <v>194</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I101" s="21" t="s">
         <v>195</v>
@@ -8681,7 +8681,7 @@
         <v>100</v>
       </c>
       <c r="L101" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -8702,7 +8702,7 @@
         <v>149</v>
       </c>
       <c r="H102" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I102" s="21" t="s">
         <v>150</v>
@@ -8714,7 +8714,7 @@
         <v>100</v>
       </c>
       <c r="L102" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -8732,7 +8732,7 @@
         <v>154</v>
       </c>
       <c r="H103" s="19" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I103" s="21" t="s">
         <v>152</v>
@@ -8744,12 +8744,12 @@
         <v>100</v>
       </c>
       <c r="L103" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="18" t="s">
-        <v>410</v>
+        <v>608</v>
       </c>
       <c r="C104" s="14"/>
       <c r="D104" s="7">
@@ -8762,7 +8762,7 @@
         <v>151</v>
       </c>
       <c r="H104" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I104" s="21" t="s">
         <v>152</v>
@@ -8774,7 +8774,7 @@
         <v>100</v>
       </c>
       <c r="L104" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -8792,7 +8792,7 @@
         <v>153</v>
       </c>
       <c r="H105" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I105" s="21" t="s">
         <v>152</v>
@@ -8804,12 +8804,12 @@
         <v>100</v>
       </c>
       <c r="L105" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C106" s="14"/>
       <c r="D106" s="7">
@@ -8822,7 +8822,7 @@
         <v>155</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I106" s="21" t="s">
         <v>156</v>
@@ -8834,7 +8834,7 @@
         <v>100</v>
       </c>
       <c r="L106" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -8855,7 +8855,7 @@
         <v>161</v>
       </c>
       <c r="H107" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I107" s="21" t="s">
         <v>160</v>
@@ -8867,12 +8867,12 @@
         <v>100</v>
       </c>
       <c r="L107" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C108" s="14"/>
       <c r="D108" s="7">
@@ -8885,7 +8885,7 @@
         <v>157</v>
       </c>
       <c r="H108" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I108" s="21" t="s">
         <v>158</v>
@@ -8897,12 +8897,12 @@
         <v>100</v>
       </c>
       <c r="L108" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C109" s="14"/>
       <c r="D109" s="7">
@@ -8915,7 +8915,7 @@
         <v>159</v>
       </c>
       <c r="H109" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I109" s="21" t="s">
         <v>160</v>
@@ -8927,12 +8927,12 @@
         <v>100</v>
       </c>
       <c r="L109" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C110" s="13"/>
       <c r="D110" s="7">
@@ -8948,7 +8948,7 @@
         <v>162</v>
       </c>
       <c r="H110" s="19" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I110" s="21" t="s">
         <v>163</v>
@@ -8960,12 +8960,12 @@
         <v>100</v>
       </c>
       <c r="L110" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C111" s="14"/>
       <c r="D111" s="7">
@@ -8978,7 +8978,7 @@
         <v>166</v>
       </c>
       <c r="H111" s="19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I111" s="21" t="s">
         <v>167</v>
@@ -8990,12 +8990,12 @@
         <v>100</v>
       </c>
       <c r="L111" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C112" s="14"/>
       <c r="D112" s="7">
@@ -9008,7 +9008,7 @@
         <v>170</v>
       </c>
       <c r="H112" s="19" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I112" s="21" t="s">
         <v>169</v>
@@ -9020,12 +9020,12 @@
         <v>100</v>
       </c>
       <c r="L112" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C113" s="14"/>
       <c r="D113" s="7">
@@ -9038,7 +9038,7 @@
         <v>168</v>
       </c>
       <c r="H113" s="19" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I113" s="21" t="s">
         <v>169</v>
@@ -9050,12 +9050,12 @@
         <v>100</v>
       </c>
       <c r="L113" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C114" s="14"/>
       <c r="E114" s="7">
@@ -9068,7 +9068,7 @@
         <v>188</v>
       </c>
       <c r="H114" s="19" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I114" s="21" t="s">
         <v>189</v>
@@ -9080,12 +9080,12 @@
         <v>100</v>
       </c>
       <c r="L114" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C115" s="14"/>
       <c r="E115" s="7">
@@ -9098,7 +9098,7 @@
         <v>197</v>
       </c>
       <c r="H115" s="19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I115" s="21" t="s">
         <v>198</v>
@@ -9110,12 +9110,12 @@
         <v>100</v>
       </c>
       <c r="L115" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C116" s="14"/>
       <c r="D116" s="7">
@@ -9131,7 +9131,7 @@
         <v>199</v>
       </c>
       <c r="H116" s="19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I116" s="21" t="s">
         <v>200</v>
@@ -9143,7 +9143,7 @@
         <v>100</v>
       </c>
       <c r="L116" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -9164,7 +9164,7 @@
         <v>173</v>
       </c>
       <c r="H117" s="19" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I117" s="21" t="s">
         <v>174</v>
@@ -9176,12 +9176,12 @@
         <v>100</v>
       </c>
       <c r="L117" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C118" s="14"/>
       <c r="D118" s="7">
@@ -9194,7 +9194,7 @@
         <v>178</v>
       </c>
       <c r="H118" s="19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I118" s="21" t="s">
         <v>174</v>
@@ -9206,12 +9206,12 @@
         <v>100</v>
       </c>
       <c r="L118" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C119" s="15">
         <v>1</v>
@@ -9229,7 +9229,7 @@
         <v>175</v>
       </c>
       <c r="H119" s="19" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I119" s="21" t="s">
         <v>174</v>
@@ -9241,12 +9241,12 @@
         <v>100</v>
       </c>
       <c r="L119" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C120" s="14"/>
       <c r="D120" s="7">
@@ -9259,7 +9259,7 @@
         <v>176</v>
       </c>
       <c r="H120" s="19" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I120" s="21" t="s">
         <v>174</v>
@@ -9271,12 +9271,12 @@
         <v>100</v>
       </c>
       <c r="L120" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C121" s="14"/>
       <c r="D121" s="7">
@@ -9289,7 +9289,7 @@
         <v>177</v>
       </c>
       <c r="H121" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I121" s="21" t="s">
         <v>174</v>
@@ -9301,7 +9301,7 @@
         <v>100</v>
       </c>
       <c r="L121" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -9321,7 +9321,7 @@
         <v>145</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I122" s="21" t="s">
         <v>146</v>
@@ -9333,7 +9333,7 @@
         <v>100</v>
       </c>
       <c r="L122" s="18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -9356,7 +9356,7 @@
         <v>202</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I123" s="4" t="s">
         <v>203</v>
@@ -9385,7 +9385,7 @@
         <v>205</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I124" s="4" t="s">
         <v>206</v>
@@ -9402,7 +9402,7 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C125" s="15">
         <v>3</v>
@@ -9414,7 +9414,7 @@
         <v>208</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I125" s="4" t="s">
         <v>209</v>
@@ -9431,7 +9431,7 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C126" s="15">
         <v>1</v>
@@ -9443,7 +9443,7 @@
         <v>211</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I126" s="4" t="s">
         <v>212</v>
@@ -9460,19 +9460,19 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="18" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C127" s="15">
         <v>2</v>
       </c>
       <c r="F127" s="22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G127" s="18" t="s">
         <v>213</v>
       </c>
       <c r="H127" s="19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I127" s="21" t="s">
         <v>214</v>
@@ -9484,7 +9484,7 @@
         <v>100</v>
       </c>
       <c r="L127" s="25" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -9505,7 +9505,7 @@
         <v>217</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I128" s="21" t="s">
         <v>216</v>
@@ -9517,12 +9517,12 @@
         <v>100</v>
       </c>
       <c r="L128" s="18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C129" s="14"/>
       <c r="E129" s="7">
@@ -9535,7 +9535,7 @@
         <v>218</v>
       </c>
       <c r="H129" s="19" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I129" s="21" t="s">
         <v>216</v>
@@ -9547,12 +9547,12 @@
         <v>100</v>
       </c>
       <c r="L129" s="18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C130" s="14"/>
       <c r="E130" s="7">
@@ -9565,7 +9565,7 @@
         <v>215</v>
       </c>
       <c r="H130" s="19" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I130" s="21" t="s">
         <v>216</v>
@@ -9577,7 +9577,7 @@
         <v>100</v>
       </c>
       <c r="L130" s="18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -9600,7 +9600,7 @@
         <v>219</v>
       </c>
       <c r="H131" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I131" s="21" t="s">
         <v>220</v>
@@ -9612,12 +9612,12 @@
         <v>100</v>
       </c>
       <c r="L131" s="18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C132" s="15">
         <v>1</v>
@@ -9629,7 +9629,7 @@
         <v>221</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I132" s="4" t="s">
         <v>222</v>
@@ -9659,7 +9659,7 @@
         <v>224</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I133" s="4" t="s">
         <v>225</v>
@@ -9671,24 +9671,24 @@
         <v>100</v>
       </c>
       <c r="L133" s="25" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C134" s="15">
         <v>1</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>226</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I134" s="4" t="s">
         <v>227</v>
@@ -9705,7 +9705,7 @@
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C135" s="15">
         <v>2</v>
@@ -9717,7 +9717,7 @@
         <v>228</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I135" s="4" t="s">
         <v>229</v>
@@ -9734,7 +9734,7 @@
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C136" s="14"/>
       <c r="D136" s="7">
@@ -9750,7 +9750,7 @@
         <v>230</v>
       </c>
       <c r="H136" s="19" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I136" s="21" t="s">
         <v>231</v>
@@ -9762,7 +9762,7 @@
         <v>99</v>
       </c>
       <c r="L136" s="18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -9779,7 +9779,7 @@
         <v>232</v>
       </c>
       <c r="H137" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I137" s="21" t="s">
         <v>233</v>
@@ -9791,12 +9791,12 @@
         <v>100</v>
       </c>
       <c r="L137" s="18" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B138" s="7">
         <v>1</v>
@@ -9809,7 +9809,7 @@
         <v>234</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I138" s="4" t="s">
         <v>235</v>
@@ -9839,7 +9839,7 @@
         <v>236</v>
       </c>
       <c r="H139" s="19" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I139" s="21" t="s">
         <v>237</v>
@@ -9851,12 +9851,12 @@
         <v>100</v>
       </c>
       <c r="L139" s="18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B140" s="3">
         <v>29</v>

</xml_diff>